<commit_message>
Modify the repo for v4.10.1
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.10.20.40_AddDevice.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.10.20.40_AddDevice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="90" yWindow="3645" windowWidth="21615" windowHeight="9570"/>
@@ -4190,35 +4190,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -4554,7 +4526,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5117,7 +5089,7 @@
         <v>651</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>845</v>
@@ -5458,26 +5430,26 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="N3:N32">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Upgrage to Ranorex 5.3
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.10.20.40_AddDevice.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.10.20.40_AddDevice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="90" yWindow="3645" windowWidth="19440" windowHeight="9570"/>
@@ -1260,7 +1260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7687" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7686" uniqueCount="889">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3994,10 +3994,6 @@
   </si>
   <si>
     <t>Pre-condition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\\Automation-2014-11\\NformTestMain\\NformTester\\NformTester\\precondition_default.xml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4553,7 +4549,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:B23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5230,9 +5226,7 @@
       <c r="A23" s="16" t="s">
         <v>888</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>889</v>
-      </c>
+      <c r="B23" s="17"/>
       <c r="C23" s="3">
         <v>22</v>
       </c>

</xml_diff>